<commit_message>
Update Excel resource file and remove temporary backup file
</commit_message>
<xml_diff>
--- a/assets/img/Tableaudesynthèse-EpreuveE5-BTSSIO2025.xlsx
+++ b/assets/img/Tableaudesynthèse-EpreuveE5-BTSSIO2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rémy\Documents\GitHub\portfolio\assets\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FA4F6A5-64FA-4527-B9E1-EE12D1D314FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95AFE15-91D4-4242-A357-CA759FABA2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -554,98 +554,98 @@
   </cellStyleXfs>
   <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1035,496 +1035,501 @@
   </sheetPr>
   <dimension ref="A1:AQ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="70.42578125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="10"/>
-    <col min="3" max="8" width="18.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="70.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1"/>
+    <col min="3" max="8" width="18.7109375" style="1" customWidth="1"/>
     <col min="9" max="43" width="11.42578125" customWidth="1"/>
-    <col min="44" max="16384" width="10.85546875" style="10"/>
+    <col min="44" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="9"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="7" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="11" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="18" customFormat="1" ht="324.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="16" t="s">
+    <row r="7" spans="1:13" s="9" customFormat="1" ht="324.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:13" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="9" spans="1:13" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
-    </row>
-    <row r="10" spans="1:13" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
+    </row>
+    <row r="10" spans="1:13" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="26"/>
-    </row>
-    <row r="11" spans="1:13" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
-    </row>
-    <row r="12" spans="1:13" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
-    </row>
-    <row r="13" spans="1:13" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="26"/>
-    </row>
-    <row r="14" spans="1:13" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
-    </row>
-    <row r="15" spans="1:13" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
-    </row>
-    <row r="16" spans="1:13" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
-    </row>
-    <row r="17" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26"/>
-    </row>
-    <row r="18" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="26"/>
-    </row>
-    <row r="19" spans="1:8" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="1:13" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
+    </row>
+    <row r="12" spans="1:13" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
+    </row>
+    <row r="13" spans="1:13" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17"/>
+    </row>
+    <row r="14" spans="1:13" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:13" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="17"/>
+    </row>
+    <row r="16" spans="1:13" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="17"/>
+    </row>
+    <row r="17" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
+    </row>
+    <row r="19" spans="1:8" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+    </row>
+    <row r="20" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="30">
+      <c r="B20" s="21">
         <v>2024</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="26"/>
-    </row>
-    <row r="21" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
+      <c r="C20" s="16"/>
+      <c r="D20" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="30">
+      <c r="B21" s="21">
         <v>2024</v>
       </c>
-      <c r="C21" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" s="26"/>
-    </row>
-    <row r="22" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="s">
+      <c r="C21" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="17"/>
+    </row>
+    <row r="22" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B22" s="21">
         <v>2024</v>
       </c>
-      <c r="C22" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="26"/>
-    </row>
-    <row r="24" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="19"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="26"/>
-    </row>
-    <row r="25" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="19"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="26"/>
-    </row>
-    <row r="26" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="19"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="26"/>
-    </row>
-    <row r="27" spans="1:8" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="C22" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="17"/>
+    </row>
+    <row r="25" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="10"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="17"/>
+    </row>
+    <row r="26" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="17"/>
+    </row>
+    <row r="27" spans="1:8" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="20" t="s">
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+    </row>
+    <row r="28" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="G28" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="H28" s="26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
+      <c r="C28" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="26"/>
-    </row>
-    <row r="30" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20" t="s">
+      <c r="C29" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="17"/>
+    </row>
+    <row r="30" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="30">
+      <c r="B30" s="21">
         <v>2025</v>
       </c>
-      <c r="C30" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="G30" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" s="26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="20"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="26"/>
-    </row>
-    <row r="32" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="19"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="26"/>
-    </row>
-    <row r="33" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="19"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="26"/>
-    </row>
-    <row r="34" spans="1:8" s="18" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="21"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="28"/>
-    </row>
-    <row r="35" spans="1:8" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="22"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
+      <c r="C30" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="11"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="17"/>
+    </row>
+    <row r="32" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="10"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="17"/>
+    </row>
+    <row r="33" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="10"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="17"/>
+    </row>
+    <row r="34" spans="1:8" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="12"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="19"/>
+    </row>
+    <row r="35" spans="1:8" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="13"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A4:E4"/>
@@ -1532,11 +1537,6 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.196527777777778" right="0.196527777777778" top="0.196527777777778" bottom="0.196527777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>